<commit_message>
Add TestSheet Change Source.c
</commit_message>
<xml_diff>
--- a/Blackjack_TestSheet.xlsx
+++ b/Blackjack_TestSheet.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m\Documents\BlackJack_Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m\Documents\GitHub\Blackjack\Blackjack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DEE3C80-FEAD-4A8B-9EDD-67164943D540}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73087413-1B58-4ACE-BF0D-7D76DF9503C9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{F40FA4D2-840E-4ED5-B48B-DAD2F9C66780}"/>
+    <workbookView xWindow="-300" yWindow="450" windowWidth="15540" windowHeight="13590" xr2:uid="{F40FA4D2-840E-4ED5-B48B-DAD2F9C66780}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSheet" sheetId="1" r:id="rId1"/>
-    <sheet name="TestSource" sheetId="2" r:id="rId2"/>
+    <sheet name="Log" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="101">
   <si>
     <t>評価項目</t>
     <rPh sb="0" eb="2">
@@ -342,16 +342,6 @@
     <rPh sb="0" eb="2">
       <t>ドウジョウ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>プログラムの実行
-1を入力
-9を入力
-10を入力
-14を入力
-22を入力
-23を入力</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -495,64 +485,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <r>
-      <t>■下記の様なログが出て、</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="游ゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Xの値が連続していない事</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
------ shuffle test start -----
-deck = X
-deck = X
-deck = X
-.
-.
------ shuffle test end -----
-■下記のログが出ないこと
-[ERROR]shuffle failed</t>
-    </r>
-    <rPh sb="0" eb="1">
-      <t>カキ</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>ヨウ</t>
-    </rPh>
-    <rPh sb="7" eb="8">
-      <t>デ</t>
-    </rPh>
-    <rPh sb="12" eb="13">
-      <t>アタイ</t>
-    </rPh>
-    <rPh sb="16" eb="18">
-      <t>レンゾク</t>
-    </rPh>
-    <rPh sb="86" eb="88">
-      <t>カキ</t>
-    </rPh>
-    <rPh sb="92" eb="93">
-      <t>デ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>s_dealerDrawCountが正しく設定されていること</t>
     <rPh sb="18" eb="19">
       <t>タダ</t>
@@ -708,16 +640,6 @@
     <t>プログラムの実行
 0を入力
 9を入力
-13を入力
-22を入力
-0を入力
-0を入力</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>プログラムの実行
-0を入力
-9を入力
 22を入力
 23を入力
 0を入力 
@@ -733,88 +655,6 @@
 22を入力
 0を入力 
 0を入力 </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">プログラムの実行
-0を入力
-9を入力
-10を入力
-11を入力
-0を入力
-0を入力 </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <r>
-      <t>■下記の様なログが表示されること
-result = 2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="游ゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> OK!!!</t>
-    </r>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">■下記の様なログが表示されること
-result = 2 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="游ゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>OK!!!</t>
-    </r>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">■下記の様なログが表示されること
-result = 1 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="游ゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>OK!!!</t>
-    </r>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">■下記の様なログが表示されること
-result = 0 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="游ゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>OK!!!</t>
-    </r>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -953,10 +793,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>https://repl.it/@ishinored/TragicAmbitiousIrcbot</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>結果</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1046,18 +882,156 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>無し</t>
+    <t>OK</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>プログラムの実行
+1を入力
+9を入力
+10を入力
+14を入力
+22を入力
+23を入力
+yを入力</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">プログラムの実行
+9を入力
+10を入力
+0を入力
+11を入力
+0を入力
+0を入力 </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OK
+※期待ログが二回出力されてしまう</t>
+    <rPh sb="4" eb="6">
+      <t>キタイ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ニカイ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>シュツリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>■下記の様なログが出て、Xの値が連続していない事
+----- shuffle test start -----
+deck = X
+deck = X
+deck = X
+.
+.
+----- shuffle test end -----
+■下記のログが出ないこと
+[ERROR]shuffle failed</t>
     <rPh sb="0" eb="1">
-      <t>ナ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
+      <t>カキ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ヨウ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>アタイ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>レンゾク</t>
+    </rPh>
+    <rPh sb="86" eb="88">
+      <t>カキ</t>
+    </rPh>
+    <rPh sb="92" eb="93">
+      <t>デ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>■下記の様なログが表示されること
+result = 2 OK!!!</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>■下記の様なログが表示されること
+result = 1 OK!!!</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>■下記の様なログが表示されること
+result = 0 OK!!!</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>4.png</t>
+  </si>
+  <si>
+    <t>2.png</t>
+  </si>
+  <si>
+    <t>3.png</t>
+  </si>
+  <si>
+    <t>5.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>6_1.png
+6_2.png
+6_3.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>7.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>8.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>9.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>10.png</t>
+  </si>
+  <si>
+    <t>11.png</t>
+  </si>
+  <si>
+    <t>12.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>13.png</t>
+  </si>
+  <si>
+    <t>14.png</t>
+  </si>
+  <si>
+    <t>15.png</t>
+  </si>
+  <si>
+    <t>https://repl.it/@ishinored/LatestFewMultiprocessing-1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1092,16 +1066,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="游ゴシック"/>
-      <family val="2"/>
+      <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="游ゴシック"/>
       <family val="3"/>
       <charset val="128"/>
@@ -1110,16 +1085,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="游ゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="游ゴシック"/>
       <family val="3"/>
       <charset val="128"/>
@@ -1152,7 +1118,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1334,39 +1300,11 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1380,117 +1318,87 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1508,6 +1416,79 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>457200</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>85725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2049" name="Object 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2049"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{671835DC-EB94-4BA5-BF04-3E33D97D0313}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd type="none" w="med" len="med"/>
+            </a:ln>
+            <a:effectLst/>
+            <a:extLst>
+              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+                <a14:hiddenEffects>
+                  <a:effectLst>
+                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                      <a:srgbClr val="808080"/>
+                    </a:outerShdw>
+                  </a:effectLst>
+                </a14:hiddenEffects>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1807,467 +1788,565 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{294E2140-17E4-4AE9-844E-5B046F72641B}">
-  <dimension ref="B2:G40"/>
+  <dimension ref="B2:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="3.25" customWidth="1"/>
-    <col min="2" max="2" width="67.5" customWidth="1"/>
-    <col min="3" max="3" width="42" customWidth="1"/>
-    <col min="4" max="4" width="66.75" customWidth="1"/>
-    <col min="5" max="5" width="8.625" customWidth="1"/>
-    <col min="6" max="6" width="35.125" customWidth="1"/>
+    <col min="1" max="1" width="3.25" style="4" customWidth="1"/>
+    <col min="2" max="2" width="67.5" style="4" customWidth="1"/>
+    <col min="3" max="3" width="42" style="4" customWidth="1"/>
+    <col min="4" max="4" width="66.75" style="4" customWidth="1"/>
+    <col min="5" max="5" width="8.625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="35.125" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="2:6" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="4"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B3" t="s">
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B5" t="s">
+      <c r="C5" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B7" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B8" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="11"/>
+    </row>
+    <row r="9" spans="2:6" ht="206.25" x14ac:dyDescent="0.4">
+      <c r="B9" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="168.75" x14ac:dyDescent="0.4">
+      <c r="B10" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="131.25" x14ac:dyDescent="0.4">
+      <c r="B11" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="150" x14ac:dyDescent="0.4">
+      <c r="B12" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B13" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="18"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B14" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="21"/>
+    </row>
+    <row r="15" spans="2:6" ht="187.5" x14ac:dyDescent="0.4">
+      <c r="B15" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="168.75" x14ac:dyDescent="0.4">
+      <c r="B16" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C16" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B17" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="21"/>
+    </row>
+    <row r="18" spans="2:6" ht="131.25" x14ac:dyDescent="0.4">
+      <c r="B18" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="104.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="B20" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="B21" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="B22" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="B23" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="B24" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="B25" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B26" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="21"/>
+    </row>
+    <row r="27" spans="2:6" ht="131.25" x14ac:dyDescent="0.4">
+      <c r="B27" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B28" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="21"/>
+    </row>
+    <row r="29" spans="2:6" ht="150" x14ac:dyDescent="0.4">
+      <c r="B29" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" ht="150" x14ac:dyDescent="0.4">
+      <c r="B30" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" ht="150" x14ac:dyDescent="0.4">
+      <c r="B31" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B32" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="21"/>
+    </row>
+    <row r="33" spans="2:6" ht="150" x14ac:dyDescent="0.4">
+      <c r="B33" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="23" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B7" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="26" t="s">
+      <c r="D33" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F33" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" ht="150" x14ac:dyDescent="0.4">
+      <c r="B34" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" ht="131.25" x14ac:dyDescent="0.4">
+      <c r="B35" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F35" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" ht="131.25" x14ac:dyDescent="0.4">
+      <c r="B36" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="F7" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B8" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="2:7" ht="206.25" x14ac:dyDescent="0.4">
-      <c r="B9" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="15"/>
-    </row>
-    <row r="10" spans="2:7" ht="168.75" x14ac:dyDescent="0.4">
-      <c r="B10" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="15"/>
-    </row>
-    <row r="11" spans="2:7" ht="131.25" x14ac:dyDescent="0.4">
-      <c r="B11" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="15"/>
-    </row>
-    <row r="12" spans="2:7" ht="150" x14ac:dyDescent="0.4">
-      <c r="B12" s="25" t="s">
+      <c r="D36" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="E36" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E12" s="27"/>
-      <c r="F12" s="15"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B13" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="9"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B14" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="36"/>
-    </row>
-    <row r="15" spans="2:7" ht="187.5" x14ac:dyDescent="0.4">
-      <c r="B15" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="28"/>
-      <c r="F15" s="15"/>
-    </row>
-    <row r="16" spans="2:7" ht="168.75" x14ac:dyDescent="0.4">
-      <c r="B16" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="E16" s="27"/>
-      <c r="F16" s="15"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B17" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="36"/>
-    </row>
-    <row r="18" spans="2:6" ht="131.25" x14ac:dyDescent="0.4">
-      <c r="B18" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" s="27"/>
-      <c r="F18" s="15"/>
-    </row>
-    <row r="19" spans="2:6" ht="104.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E19" s="27"/>
-      <c r="F19" s="15"/>
-    </row>
-    <row r="20" spans="2:6" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="B20" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="27"/>
-      <c r="F20" s="15"/>
-    </row>
-    <row r="21" spans="2:6" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="B21" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" s="27"/>
-      <c r="F21" s="15"/>
-    </row>
-    <row r="22" spans="2:6" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="B22" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E22" s="27"/>
-      <c r="F22" s="15"/>
-    </row>
-    <row r="23" spans="2:6" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="B23" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="27"/>
-      <c r="F23" s="15"/>
-    </row>
-    <row r="24" spans="2:6" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="B24" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="27"/>
-      <c r="F24" s="15"/>
-    </row>
-    <row r="25" spans="2:6" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="B25" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E25" s="27"/>
-      <c r="F25" s="15"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B26" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="C26" s="35"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="36"/>
-    </row>
-    <row r="27" spans="2:6" ht="131.25" x14ac:dyDescent="0.4">
-      <c r="B27" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D27" s="2" t="s">
+      <c r="F36" s="16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B37" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="21"/>
+    </row>
+    <row r="38" spans="2:6" ht="131.25" x14ac:dyDescent="0.4">
+      <c r="B38" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="D38" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="28"/>
-      <c r="F27" s="15"/>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B28" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28" s="35"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="36"/>
-    </row>
-    <row r="29" spans="2:6" ht="150" x14ac:dyDescent="0.4">
-      <c r="B29" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E29" s="29"/>
-      <c r="F29" s="15"/>
-    </row>
-    <row r="30" spans="2:6" ht="150" x14ac:dyDescent="0.4">
-      <c r="B30" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E30" s="29"/>
-      <c r="F30" s="15"/>
-    </row>
-    <row r="31" spans="2:6" ht="150" x14ac:dyDescent="0.4">
-      <c r="B31" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E31" s="28"/>
-      <c r="F31" s="15"/>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B32" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="C32" s="35"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="36"/>
-    </row>
-    <row r="33" spans="2:6" ht="131.25" x14ac:dyDescent="0.4">
-      <c r="B33" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E33" s="28"/>
-      <c r="F33" s="15"/>
-    </row>
-    <row r="34" spans="2:6" ht="150" x14ac:dyDescent="0.4">
-      <c r="B34" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E34" s="28"/>
-      <c r="F34" s="15"/>
-    </row>
-    <row r="35" spans="2:6" ht="131.25" x14ac:dyDescent="0.4">
-      <c r="B35" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E35" s="28"/>
-      <c r="F35" s="15"/>
-    </row>
-    <row r="36" spans="2:6" ht="131.25" x14ac:dyDescent="0.4">
-      <c r="B36" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E36" s="28"/>
-      <c r="F36" s="15"/>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B37" s="34" t="s">
+      <c r="E38" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F38" s="16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" ht="131.25" x14ac:dyDescent="0.4">
+      <c r="B39" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="C37" s="35"/>
-      <c r="D37" s="35"/>
-      <c r="E37" s="35"/>
-      <c r="F37" s="36"/>
-    </row>
-    <row r="38" spans="2:6" ht="131.25" x14ac:dyDescent="0.4">
-      <c r="B38" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D38" s="2" t="s">
+      <c r="D39" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E38" s="28"/>
-      <c r="F38" s="15"/>
-    </row>
-    <row r="39" spans="2:6" ht="131.25" x14ac:dyDescent="0.4">
-      <c r="B39" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D39" s="2" t="s">
+      <c r="E39" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F39" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" ht="150.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B40" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D40" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E39" s="28"/>
-      <c r="F39" s="15"/>
-    </row>
-    <row r="40" spans="2:6" ht="132" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B40" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C40" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="D40" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="E40" s="30"/>
-      <c r="F40" s="24"/>
+      <c r="E40" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F40" s="16" t="s">
+        <v>96</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2283,7 +2362,7 @@
   <phoneticPr fontId="1"/>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{39E55410-8CC9-45FC-9159-0C29F2B3CC56}"/>
-    <hyperlink ref="C5" r:id="rId2" xr:uid="{946C4D89-E9DE-4109-B090-D30EB1982B49}"/>
+    <hyperlink ref="C5" r:id="rId2" xr:uid="{CE6B0C2D-8555-495B-925D-78F1E0A5826E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -2291,21 +2370,46 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A46E818-2038-473D-998C-6A670D08BA60}">
-  <dimension ref="B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A46E818-2038-473D-998C-6A670D08BA60}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
-  <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <oleObjects>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="パッケージャー シェル オブジェクト" dvAspect="DVASPECT_ICON" shapeId="2049" r:id="rId4">
+          <objectPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>457200</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="パッケージャー シェル オブジェクト" dvAspect="DVASPECT_ICON" shapeId="2049" r:id="rId4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </oleObjects>
 </worksheet>
 </file>
</xml_diff>